<commit_message>
update vocabulary and MeasurementOrFact table
</commit_message>
<xml_diff>
--- a/Data/MetadataDictionary_v1.xlsx
+++ b/Data/MetadataDictionary_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rscully\Documents\Projects\Habitat Data Sharing\2019_2020\Code\Stream-Monitoring-Data-Exchange-Specifications\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B63E159-2468-4575-BECC-3DF96E104325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0290F47-681E-464A-BC22-22138D682BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{612D857E-CB7D-4F80-AB73-368B543E7FF3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{612D857E-CB7D-4F80-AB73-368B543E7FF3}"/>
   </bookViews>
   <sheets>
     <sheet name="MetadataDict" sheetId="2" r:id="rId1"/>
@@ -322,7 +322,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="396">
   <si>
     <t>tblname</t>
   </si>
@@ -1507,6 +1507,9 @@
   </si>
   <si>
     <t>The original type of data assigned in the source dataset as read by computer software.</t>
+  </si>
+  <si>
+    <t>measurmentTypeID</t>
   </si>
 </sst>
 </file>
@@ -1941,16 +1944,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E6029B-A891-4391-9A91-8B6BC1C75C07}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23:B29"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" customWidth="1"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.26953125" customWidth="1"/>
     <col min="3" max="3" width="43.54296875" style="3" customWidth="1"/>
     <col min="4" max="8" width="10.1796875" customWidth="1"/>
@@ -2013,7 +2017,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>299</v>
       </c>
@@ -2027,7 +2031,7 @@
       <c r="M2" s="3"/>
       <c r="O2"/>
     </row>
-    <row r="3" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>299</v>
       </c>
@@ -2054,7 +2058,7 @@
       </c>
       <c r="O3"/>
     </row>
-    <row r="4" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>299</v>
       </c>
@@ -2084,7 +2088,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>299</v>
       </c>
@@ -2117,7 +2121,7 @@
       </c>
       <c r="O5"/>
     </row>
-    <row r="6" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>299</v>
       </c>
@@ -2152,7 +2156,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>299</v>
       </c>
@@ -2181,7 +2185,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>299</v>
       </c>
@@ -2205,7 +2209,7 @@
       </c>
       <c r="O8"/>
     </row>
-    <row r="9" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>299</v>
       </c>
@@ -2235,7 +2239,7 @@
       </c>
       <c r="O9"/>
     </row>
-    <row r="10" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>299</v>
       </c>
@@ -2264,7 +2268,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>299</v>
       </c>
@@ -2293,7 +2297,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -2304,7 +2308,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -2324,7 +2328,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -2353,7 +2357,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -2379,7 +2383,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -2408,7 +2412,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -2437,7 +2441,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -2460,7 +2464,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>245</v>
       </c>
@@ -2495,7 +2499,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -2524,7 +2528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" ht="63.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -2538,7 +2542,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -2561,7 +2565,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2599,7 +2603,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2628,7 +2632,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -2663,7 +2667,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" ht="44.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -2695,7 +2699,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" ht="33.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2727,7 +2731,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -2759,7 +2763,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -2868,7 +2872,7 @@
         <v>374</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>395</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>345</v>
@@ -2917,7 +2921,7 @@
         <v>374</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>319</v>
@@ -2941,7 +2945,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>296</v>
       </c>
@@ -2953,7 +2957,7 @@
       </c>
       <c r="O36"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>296</v>
       </c>
@@ -2971,7 +2975,7 @@
       </c>
       <c r="O37"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>296</v>
       </c>
@@ -2989,7 +2993,7 @@
       </c>
       <c r="O38"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>296</v>
       </c>
@@ -3009,7 +3013,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>296</v>
       </c>
@@ -3027,7 +3031,7 @@
       </c>
       <c r="O40"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>296</v>
       </c>
@@ -3047,7 +3051,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>296</v>
       </c>
@@ -3073,7 +3077,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>296</v>
       </c>
@@ -3093,7 +3097,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>296</v>
       </c>
@@ -3117,7 +3121,7 @@
       </c>
       <c r="O44"/>
     </row>
-    <row r="45" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" ht="33" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>296</v>
       </c>
@@ -3141,7 +3145,7 @@
       </c>
       <c r="O45"/>
     </row>
-    <row r="46" spans="1:16" ht="87" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>297</v>
       </c>
@@ -3153,7 +3157,7 @@
       </c>
       <c r="O46"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>297</v>
       </c>
@@ -3174,7 +3178,7 @@
       </c>
       <c r="O47"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>297</v>
       </c>
@@ -3195,7 +3199,7 @@
       </c>
       <c r="O48"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>297</v>
       </c>
@@ -3216,7 +3220,7 @@
       </c>
       <c r="O49"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>297</v>
       </c>
@@ -3237,7 +3241,7 @@
       </c>
       <c r="O50"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>297</v>
       </c>
@@ -3258,7 +3262,7 @@
       </c>
       <c r="O51"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>297</v>
       </c>
@@ -3285,7 +3289,7 @@
       </c>
       <c r="O52"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>297</v>
       </c>
@@ -3306,7 +3310,7 @@
       </c>
       <c r="O53"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>297</v>
       </c>
@@ -3333,7 +3337,7 @@
       </c>
       <c r="O54"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>297</v>
       </c>
@@ -3357,7 +3361,7 @@
       </c>
       <c r="O55"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>297</v>
       </c>
@@ -3383,6 +3387,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O56" xr:uid="{41E6029B-A891-4391-9A91-8B6BC1C75C07}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="MeasurementOrFact"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:O11">
       <sortCondition ref="B1:B45"/>
     </sortState>
@@ -4447,7 +4456,7 @@
       </c>
       <c r="B55" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>146</v>
@@ -4471,7 +4480,7 @@
       </c>
       <c r="B56" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>148</v>
@@ -4495,7 +4504,7 @@
       </c>
       <c r="B57" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>150</v>
@@ -4519,7 +4528,7 @@
       </c>
       <c r="B58" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>152</v>
@@ -4543,7 +4552,7 @@
       </c>
       <c r="B59" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>154</v>
@@ -4567,7 +4576,7 @@
       </c>
       <c r="B60" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>158</v>
@@ -4591,7 +4600,7 @@
       </c>
       <c r="B61" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>160</v>
@@ -4615,7 +4624,7 @@
       </c>
       <c r="B62" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>162</v>
@@ -4639,7 +4648,7 @@
       </c>
       <c r="B63" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>164</v>
@@ -4663,7 +4672,7 @@
       </c>
       <c r="B64" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>166</v>
@@ -4687,7 +4696,7 @@
       </c>
       <c r="B65" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>168</v>
@@ -4711,7 +4720,7 @@
       </c>
       <c r="B66" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>170</v>
@@ -4735,7 +4744,7 @@
       </c>
       <c r="B67" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>172</v>
@@ -4759,7 +4768,7 @@
       </c>
       <c r="B68" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>174</v>
@@ -4783,7 +4792,7 @@
       </c>
       <c r="B69" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>176</v>
@@ -4807,7 +4816,7 @@
       </c>
       <c r="B70" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>178</v>
@@ -4831,7 +4840,7 @@
       </c>
       <c r="B71" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>180</v>
@@ -4855,7 +4864,7 @@
       </c>
       <c r="B72" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>182</v>
@@ -4879,7 +4888,7 @@
       </c>
       <c r="B73" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>184</v>
@@ -4903,7 +4912,7 @@
       </c>
       <c r="B74" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>186</v>
@@ -4927,7 +4936,7 @@
       </c>
       <c r="B75" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>188</v>
@@ -4951,7 +4960,7 @@
       </c>
       <c r="B76" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>190</v>
@@ -4975,7 +4984,7 @@
       </c>
       <c r="B77" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>192</v>
@@ -4999,7 +5008,7 @@
       </c>
       <c r="B78" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>194</v>
@@ -5023,7 +5032,7 @@
       </c>
       <c r="B79" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>196</v>
@@ -5047,7 +5056,7 @@
       </c>
       <c r="B80" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>198</v>
@@ -5071,7 +5080,7 @@
       </c>
       <c r="B81" s="1" t="str">
         <f>MetadataDict!$B$35</f>
-        <v>term</v>
+        <v>measurementType</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>200</v>
@@ -5227,7 +5236,7 @@
       </c>
       <c r="B89" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C89" s="4">
         <v>35</v>
@@ -5287,7 +5296,7 @@
       </c>
       <c r="B92" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C92" s="4">
         <v>36</v>
@@ -5347,7 +5356,7 @@
       </c>
       <c r="B95" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C95" s="4">
         <v>37</v>
@@ -5407,7 +5416,7 @@
       </c>
       <c r="B98" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C98" s="4">
         <v>38</v>
@@ -5467,7 +5476,7 @@
       </c>
       <c r="B101" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C101" s="4">
         <v>39</v>
@@ -5566,7 +5575,7 @@
       </c>
       <c r="B106" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C106" s="4">
         <v>41</v>
@@ -5632,7 +5641,7 @@
       </c>
       <c r="B109" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C109" s="4">
         <v>42</v>
@@ -5692,7 +5701,7 @@
       </c>
       <c r="B112" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C112" s="4">
         <v>43</v>
@@ -5734,7 +5743,7 @@
       </c>
       <c r="B114" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C114" s="4">
         <v>44</v>
@@ -5776,7 +5785,7 @@
       </c>
       <c r="B116" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C116" s="4">
         <v>46</v>
@@ -5824,7 +5833,7 @@
       </c>
       <c r="B118" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C118" s="4">
         <v>47</v>
@@ -5866,7 +5875,7 @@
       </c>
       <c r="B120" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C120" s="4">
         <v>48</v>
@@ -5908,7 +5917,7 @@
       </c>
       <c r="B122" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C122" s="4">
         <v>49</v>
@@ -6298,7 +6307,7 @@
       </c>
       <c r="B142" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C142" s="4">
         <v>50</v>
@@ -6340,7 +6349,7 @@
       </c>
       <c r="B144" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C144" s="4">
         <v>51</v>
@@ -6382,7 +6391,7 @@
       </c>
       <c r="B146" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C146" s="4">
         <v>52</v>
@@ -6424,7 +6433,7 @@
       </c>
       <c r="B148" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C148" s="4">
         <v>53</v>
@@ -6472,7 +6481,7 @@
       </c>
       <c r="B150" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C150" s="4">
         <v>54</v>
@@ -6520,7 +6529,7 @@
       </c>
       <c r="B152" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C152" s="4">
         <v>55</v>
@@ -6568,7 +6577,7 @@
       </c>
       <c r="B154" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C154" s="4">
         <v>56</v>
@@ -6616,7 +6625,7 @@
       </c>
       <c r="B156" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C156" s="4">
         <v>57</v>
@@ -6664,7 +6673,7 @@
       </c>
       <c r="B158" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C158" s="2">
         <v>58</v>
@@ -6707,7 +6716,7 @@
       </c>
       <c r="B160" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C160" s="4">
         <v>59</v>
@@ -6749,7 +6758,7 @@
       </c>
       <c r="B162" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C162" s="4">
         <v>60</v>
@@ -6791,7 +6800,7 @@
       </c>
       <c r="B164" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C164" s="4">
         <v>61</v>
@@ -6833,7 +6842,7 @@
       </c>
       <c r="B166" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C166" s="4">
         <v>62</v>
@@ -6875,7 +6884,7 @@
       </c>
       <c r="B168" s="1" t="str">
         <f>MetadataDict!$B$33</f>
-        <v>termID</v>
+        <v>measurmentTypeID</v>
       </c>
       <c r="C168" s="4">
         <v>63</v>
@@ -8098,16 +8107,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F29970C-55C3-4834-9A3F-8E46C108106D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="3618cbaa-901d-4c6b-9f1a-f53e3aa15701"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>